<commit_message>
fixing bug ui - add the 404 page
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log houssin mhamdi.xlsx
+++ b/DTT-Assessment-Hour-Log houssin mhamdi.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <r>
       <rPr>
@@ -136,6 +136,24 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>bug fixing (ui styling)</t>
+  </si>
+  <si>
+    <t>29/08/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix all the bug that i faced in the ui </t>
+  </si>
+  <si>
+    <t xml:space="preserve">add the 404 page </t>
+  </si>
+  <si>
+    <t>31/08/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add 404 page if the rout not exisit  alos in details page in the id not correct redirect him to home page </t>
   </si>
   <si>
     <t>Total amount of hours</t>
@@ -965,19 +983,37 @@
       <c r="F15" s="10"/>
     </row>
     <row r="16" ht="16.5" customHeight="1">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
+      <c r="A16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>38</v>
+      </c>
       <c r="E16" s="15"/>
       <c r="F16" s="10"/>
     </row>
     <row r="17" ht="16.5" customHeight="1">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="15"/>
+      <c r="A17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="F17" s="10"/>
     </row>
     <row r="18" ht="16.5" customHeight="1">
@@ -1078,11 +1114,11 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="24" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B30" s="25">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="23"/>

</xml_diff>